<commit_message>
updated the dose_response script
</commit_message>
<xml_diff>
--- a/data/grouped_bars/proxe_supp.xlsx
+++ b/data/grouped_bars/proxe_supp.xlsx
@@ -13,11 +13,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Construct</t>
   </si>
   <si>
+    <t xml:space="preserve"> - SENSOR_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - SENSOR_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - SENSOR_3</t>
+  </si>
+  <si>
     <t xml:space="preserve"> + SENSOR_1</t>
   </si>
   <si>
@@ -27,15 +36,6 @@
     <t xml:space="preserve"> + SENSOR_3</t>
   </si>
   <si>
-    <t xml:space="preserve"> - SENSOR_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - SENSOR_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - SENSOR_3</t>
-  </si>
-  <si>
     <t>REFERENCE</t>
   </si>
   <si>
@@ -75,7 +75,7 @@
     <t>Save location</t>
   </si>
   <si>
-    <t>Generalist Biosensors Response to Benzylisoquinoline Alkaloids</t>
+    <t>Promoter activity with and without cognate biosensor</t>
   </si>
   <si>
     <t>Biosensor</t>
@@ -84,22 +84,10 @@
     <t>(RFU/OD)</t>
   </si>
   <si>
-    <t>#757575</t>
-  </si>
-  <si>
-    <t>#7814fc</t>
-  </si>
-  <si>
-    <t>#d9ce00</t>
-  </si>
-  <si>
-    <t>#ff1900</t>
-  </si>
-  <si>
-    <t>#25de00</t>
-  </si>
-  <si>
-    <t>#ff910a</t>
+    <t>#6e6e6e</t>
+  </si>
+  <si>
+    <t>#1fde0d</t>
   </si>
 </sst>
 </file>
@@ -144,21 +132,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -425,163 +410,163 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>389.0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>430.0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>416.0</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>23847.0</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>24298.0</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>26044.0</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>105.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>171.0</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>153.5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>136.0</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>12201.0</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>12899.0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>12939.0</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>119.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>197.0</v>
       </c>
       <c r="C4" s="6">
-        <v>185.0</v>
-      </c>
-      <c r="D4" s="6">
+        <v>197.0</v>
+      </c>
+      <c r="D4" s="5">
         <v>189.0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>19932.0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <f>AVERAGE(E4,G4)</f>
         <v>22242.5</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>24553.0</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>127.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>441.0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>424.0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>424.0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>27503.0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>27242.0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>26245.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>150.0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>146.0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>161.0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>15999.0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>16504.0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>16655.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>333.0</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>327.0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>340.0</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>18800.0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>19926.0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>19707.0</v>
       </c>
     </row>
@@ -604,184 +589,184 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0.6417000294</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>0.6798999906</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>0.6450999975</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0.5526000261</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>0.5465999842</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>0.5701000094</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>0.6345999837</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0.1995999962</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <f>AVERAGE(B3,D3)</f>
         <v>0.1833499968</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.1670999974</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.6356999874</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0.6541000009</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>0.6437000036</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.717599988</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.6143000126</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.6205000281</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.5891000032</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.4359999895</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0.4338000119</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.5360000134</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.7178999782</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.663500011</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.605799973</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.606400013</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.5070999861</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>0.4670000076</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0.4390000105</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>0.7285000086</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>0.7251999974</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0.7516000271</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.6212999821</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.6345999837</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0.6378999949</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.6888999939</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.7372999787</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.7294999957</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.6136999726</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0.6421999931</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>0.638199985</v>
       </c>
     </row>
@@ -821,13 +806,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -839,43 +824,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="D5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="11">
-      <c r="D11" s="10"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12">
-      <c r="D12" s="10"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13">
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14">
-      <c r="D14" s="10"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15">
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16">
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>